<commit_message>
[CPU]Sch update - Femto release version
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V2.0/01_RF-GEN-CPU-001/RF-GEN_CPU PL_V2.0_20200208.xlsx
+++ b/1_Schematic/Build V2.0/01_RF-GEN-CPU-001/RF-GEN_CPU PL_V2.0_20200208.xlsx
@@ -2822,7 +2822,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2834,7 +2834,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>